<commit_message>
two testcases 9 10
</commit_message>
<xml_diff>
--- a/Project/testdata/Excel.xlsx
+++ b/Project/testdata/Excel.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Pruthvi" sheetId="1" r:id="rId1"/>
+    <sheet name="Pruthvi1" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,46 +407,73 @@
       <c r="A1" t="str">
         <v>Manufacturing &amp; Processing Machinery</v>
       </c>
+      <c r="B1" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Machine-Tools.html</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Consumer Electronics</v>
       </c>
+      <c r="B2" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Engineering-Construction-Machinery.html</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Industrial Equipment &amp; Components</v>
       </c>
+      <c r="B3" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Woodworking-Machinery.html</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>Electrical &amp; Electronics</v>
       </c>
+      <c r="B4" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Plastic-Machinery.html</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
         <v>Construction &amp; Decoration</v>
       </c>
+      <c r="B5" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Metallic-Processing-Machinery.html</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Light Industry &amp; Daily Use</v>
       </c>
+      <c r="B6" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Mould.html</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>Auto, Motorcycle Parts &amp; Accessories</v>
       </c>
+      <c r="B7" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Laser-Equipment.html</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>Apparel &amp; Accessories</v>
       </c>
+      <c r="B8" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Casting-Forging.html</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
         <v>Lights &amp; Lighting</v>
       </c>
+      <c r="B9" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Agricultural-Machinery.html</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -454,7 +482,31 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Machine-Tools.html</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>/Manufacturing-Processing-Machinery-Catalog/Engineering-Construction-Machinery.html</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>